<commit_message>
public and update CSU
</commit_message>
<xml_diff>
--- a/CSU.xlsx
+++ b/CSU.xlsx
@@ -1,32 +1,154 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minhv\OneDrive\Desktop\Model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D74C1AD-5850-4256-A635-0CF2C507621A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Amortization of Intangible Assets</t>
+  </si>
+  <si>
+    <t>Foreign exchange (gain) loss</t>
+  </si>
+  <si>
+    <t>IRGA / TSS membership liability revaluation charge</t>
+  </si>
+  <si>
+    <t>Finance and other income</t>
+  </si>
+  <si>
+    <t>Bargain purchase gain</t>
+  </si>
+  <si>
+    <t>Impairment of intangible and other non-financial assets</t>
+  </si>
+  <si>
+    <t>Redeemable preferred securities expenses (income)</t>
+  </si>
+  <si>
+    <t>Finance costs</t>
+  </si>
+  <si>
+    <t>Income before income taxes</t>
+  </si>
+  <si>
+    <t>Income tax expense (recovery)</t>
+  </si>
+  <si>
+    <t>Deferred income tax expense (recovery)</t>
+  </si>
+  <si>
+    <t>Current income tax expense (recovery)</t>
+  </si>
+  <si>
+    <t>Net income (loss) attributable to</t>
+  </si>
+  <si>
+    <t>Equity holders of CSI</t>
+  </si>
+  <si>
+    <t>Non-controlling interests</t>
+  </si>
+  <si>
+    <t>Net income (loss)</t>
+  </si>
+  <si>
+    <t>Net cash flow from operating activities</t>
+  </si>
+  <si>
+    <t>Free cash flow available to shareholders</t>
+  </si>
+  <si>
+    <t>Weighted average number of shares outstanding</t>
+  </si>
+  <si>
+    <t>Basic and diluted</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Licenses</t>
+  </si>
+  <si>
+    <t>Professional services</t>
+  </si>
+  <si>
+    <t>Hardware and other</t>
+  </si>
+  <si>
+    <t>Maintenance and other recurring</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,13 +168,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +460,339 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.42578125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="1">
+        <f>+C2+1</f>
+        <v>2021</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:N2" si="0">+D2+1</f>
+        <v>2022</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <f>+SUM(C4:C7)</f>
+        <v>3969</v>
+      </c>
+      <c r="D3" s="3">
+        <f>+SUM(D4:D7)</f>
+        <v>5107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3">
+        <v>234</v>
+      </c>
+      <c r="D4" s="3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3">
+        <v>751</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>169</v>
+      </c>
+      <c r="D6" s="3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2815</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3">
+        <v>46</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3">
+        <f>+C3-C9-SUM(C11:C18)</f>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <f>+SUM(C22:C23)</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3">
+        <f>+C19-C24</f>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3">
+        <f>+SUM(C27:C28)</f>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="3">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="3">
+        <f>+C29/C36</f>
+        <v>20.660377358490567</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>